<commit_message>
Revision to the portfolios
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio - Proportional Buildout 1.31.2024.xlsx
+++ b/data/SJV Portfolio - Proportional Buildout 1.31.2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/Portfolio Inventory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6D3E0D-6293-D146-96AA-446CD830AD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC79486-CD4E-E043-B994-801FF4A3FF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="880" windowWidth="36000" windowHeight="20800" activeTab="1" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20800" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="96">
   <si>
     <t>Solar</t>
   </si>
@@ -254,9 +254,6 @@
     <t>Hydrogen Use</t>
   </si>
   <si>
-    <t>Name: Current Projects Portfolio</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -290,15 +287,6 @@
     <t>Electricity (GW)</t>
   </si>
   <si>
-    <t>Step 1: Name and Describe Your Portfolio</t>
-  </si>
-  <si>
-    <t>Description: This portfolio describes The Current Projects portfolio reflects clean energy development projects that are being planned for or under way in the SJV. This includes:
-• Anticipated electricity resource buildouts described in the IPR Busbar Study (cite) that are associated with substations located in the SJV. This includes a buildout of 13.3 GW of utility solar, 270 MW of wind, 20MW of biomass and biomethane, 7.4 GW of battery storage, and 1 GW of long-duration energy storage. We allocate biomass and biogas to feedstocks according to the relative electricity production potential of each resource, as shown in Table B.2.
-• The Lone Cypress Blue Hydrogen facility located in Kern County and scheduled to come online in 2026 and produce 30 tons of H2 per day (11,000 tons/year) (California Resources Corporation, undated)
-• The DOE Hydrogen Hub facilities located in the Central Valley. The DOE has indicated that a total of 3 MMT of hydrogen will be produced from the 7 facilities. We estimate that the SJV would produce approximately 215,000 tons of hydrogen per year, if California produced 1/7th of the DOE total, and if half of California’s production took place in the SJV as suggested by the proposed facility locations (cite). The production of hydrogen by resource type is not available for these facilities. Connelly et al. (2020) suggest that solar production potential in the SJV may be 10 times larger than biogas production potential, which may be 10 times larger than biomass production potential. Consistent with this, we assume approximately 90% of production from solar, and 9% from biomethane, and 1% from biomass. We allocate biomass and biogas to feedstocks according to the relative hydrogen production potential of each resource.</t>
-  </si>
-  <si>
     <t>Step 3: What percent of the produced hydrogen should go to transportation vs. ammonia</t>
   </si>
   <si>
@@ -408,6 +396,18 @@
   </si>
   <si>
     <t>SAF rom Biomass</t>
+  </si>
+  <si>
+    <t>Description: The Proportional portfolio reflects a buildout of energy resources in the SJV consistent with the idea that the SJV contributes to the State's energy goals proportional to its resources. That proportionality is defined differently for each feedstock to commodity pathway and should be thought of as a guiding principle rather than a strict rule.</t>
+  </si>
+  <si>
+    <t>Step 1: Name and Describe Your Portfolio and add your name</t>
+  </si>
+  <si>
+    <t>Portfolio Name: Proportional Portfolio</t>
+  </si>
+  <si>
+    <t>Created By: Nidhi Kalra (nidhi@rand.org)</t>
   </si>
 </sst>
 </file>
@@ -954,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA35989-F8F5-C645-8F8C-CB2D79A95BD0}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="133" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,15 +967,16 @@
     <col min="3" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>42</v>
       </c>
@@ -987,21 +988,26 @@
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
     </row>
-    <row r="3" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="28" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+    </row>
+    <row r="4" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -1009,12 +1015,12 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1097,7 +1103,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1170,7 +1176,7 @@
       </c>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1182,7 +1188,7 @@
       </c>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="11">
         <v>5</v>
@@ -1390,7 +1396,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1434,11 +1440,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1448,7 +1455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225537EC-F8DB-7B4E-B90C-2D6AA935C6A7}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
@@ -1462,22 +1469,22 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" t="s">
-        <v>63</v>
       </c>
       <c r="G1">
         <v>2025</v>
@@ -1545,22 +1552,22 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G2" s="18">
         <f>AA2/21</f>
@@ -1649,22 +1656,22 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G3" s="18">
         <f t="shared" ref="G3:G20" si="1">AA3/21</f>
@@ -1753,22 +1760,22 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G4" s="18">
         <f t="shared" si="1"/>
@@ -1857,22 +1864,22 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G5" s="18">
         <f t="shared" si="1"/>
@@ -1961,22 +1968,22 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G6" s="18">
         <f t="shared" si="1"/>
@@ -2065,22 +2072,22 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G7" s="18">
         <f t="shared" si="1"/>
@@ -2169,22 +2176,22 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G8" s="18">
         <f t="shared" si="1"/>
@@ -2273,22 +2280,22 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G9" s="18">
         <f t="shared" si="1"/>
@@ -2377,13 +2384,13 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -2392,7 +2399,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G10" s="18">
         <f t="shared" si="1"/>
@@ -2481,13 +2488,13 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -2496,7 +2503,7 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G11" s="18">
         <f t="shared" si="1"/>
@@ -2585,13 +2592,13 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -2600,7 +2607,7 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G12" s="18">
         <f t="shared" si="1"/>
@@ -2689,13 +2696,13 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -2704,7 +2711,7 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G13" s="18">
         <f t="shared" si="1"/>
@@ -2793,13 +2800,13 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
@@ -2808,7 +2815,7 @@
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G14" s="18">
         <f t="shared" si="1"/>
@@ -2897,13 +2904,13 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -2912,7 +2919,7 @@
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G15" s="18">
         <f t="shared" si="1"/>
@@ -3001,13 +3008,13 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -3016,7 +3023,7 @@
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G16" s="18">
         <f t="shared" si="1"/>
@@ -3105,13 +3112,13 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -3120,7 +3127,7 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G17" s="18">
         <f t="shared" si="1"/>
@@ -3209,13 +3216,13 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -3224,7 +3231,7 @@
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G18" s="18">
         <f t="shared" si="1"/>
@@ -3313,13 +3320,13 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -3328,7 +3335,7 @@
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G19" s="18">
         <f t="shared" si="1"/>
@@ -3417,13 +3424,13 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -3432,7 +3439,7 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G20" s="18">
         <f t="shared" si="1"/>
@@ -3540,10 +3547,10 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C1" s="25">
         <v>2025</v>
@@ -3614,7 +3621,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" s="25">
         <v>1</v>
@@ -3685,7 +3692,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C3" s="25">
         <v>0.5</v>
@@ -3756,7 +3763,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C4" s="25">
         <v>0.5</v>
@@ -3827,7 +3834,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C5" s="25">
         <v>1</v>
@@ -3898,7 +3905,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C6" s="25">
         <v>1</v>
@@ -3986,24 +3993,24 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="18">
         <v>654000</v>
@@ -4052,13 +4059,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -4086,7 +4093,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>480</v>
@@ -4095,10 +4102,10 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>13</v>
@@ -4139,7 +4146,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10">
         <v>0.85</v>
@@ -4188,7 +4195,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13">
         <v>0.04</v>
@@ -4212,7 +4219,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5">
         <v>140000</v>
@@ -4236,7 +4243,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -4252,7 +4259,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B16">
         <v>100</v>

</xml_diff>

<commit_message>
Reverted to biomethane category and made biomethane for h2 and elec 0
This is to hack our way to portfolio analysis while we remove biomethane as an intermediate pathway.
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio - Proportional Buildout 1.31.2024.xlsx
+++ b/data/SJV Portfolio - Proportional Buildout 1.31.2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7893D4C-76F1-9446-A009-FAA8E9D92358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D631D6F9-B607-0141-9F28-50023C835A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="880" windowWidth="36000" windowHeight="20800" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
+    <workbookView xWindow="0" yWindow="4060" windowWidth="36000" windowHeight="20800" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
   <sheets>
     <sheet name="portfolio_input" sheetId="1" r:id="rId1"/>
@@ -420,13 +420,13 @@
     <t>Proportional Portfolio</t>
   </si>
   <si>
-    <t>The Proportional portfolio reflects a buildout of energy resources in the SJV consistent with the idea that the SJV contributes to the State's energy goals proportional to its resources. That proportionality is defined differently for each feedstock to commodity pathway and should be thought of as a guiding principle rather than a strict rule.</t>
-  </si>
-  <si>
     <t>Nidhi Kalra (nidhi@rand.org)</t>
   </si>
   <si>
     <t>Metadata Value</t>
+  </si>
+  <si>
+    <t>The Proportional portfolio reflects a buildout of energy resources in the SJV consistent with the idea that the SJV contributes to the State's energy goals proportional to its resources. That proportionality is defined differently for each feedstock to commodity pathway and should be thought of as a guiding principle rather than a strict rule. THIS PORTFOLIO ONLY USES BIOGAS TO PRODUCE BIOMETHANE FOR THE GAS GRID WHILE WE UPDATE THE MODEL.</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -624,6 +624,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -633,7 +640,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA35989-F8F5-C645-8F8C-CB2D79A95BD0}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="133" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -997,35 +1003,35 @@
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
@@ -1152,7 +1158,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="23">
-        <v>2.1118012422360249E-2</v>
+        <v>3.4285714285714287E-2</v>
       </c>
       <c r="D12" s="14">
         <v>0.02</v>
@@ -1172,7 +1178,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="23">
-        <v>3.478260869565218E-3</v>
+        <v>3.0168589174800367E-3</v>
       </c>
       <c r="D13" s="13">
         <v>0.02</v>
@@ -1189,44 +1195,53 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="23">
-        <v>1.4906832298136647E-2</v>
+        <v>7</v>
+      </c>
+      <c r="C14" s="27">
+        <v>0</v>
       </c>
       <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="23">
-        <v>4.9689440993788822E-4</v>
-      </c>
-      <c r="D15" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="C15" s="21">
+        <f>D15</f>
+        <v>310000</v>
+      </c>
+      <c r="D15" s="16">
+        <v>310000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C16" s="21">
         <f>D16</f>
-        <v>310000</v>
+        <v>11000</v>
       </c>
       <c r="D16" s="16">
-        <v>310000</v>
+        <v>11000</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1234,20 +1249,19 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="21">
-        <f>D17</f>
-        <v>11000</v>
+        <v>6</v>
+      </c>
+      <c r="C17" s="24">
+        <v>120157.48031496063</v>
       </c>
       <c r="D17" s="16">
-        <v>11000</v>
+        <v>70000</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1255,10 +1269,10 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="24">
-        <v>69839.816933638445</v>
+        <v>9898.5567307519032</v>
       </c>
       <c r="D18" s="16">
         <v>70000</v>
@@ -1275,83 +1289,91 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="24">
-        <v>34840.000209458078</v>
-      </c>
-      <c r="D19" s="16">
-        <v>70000</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C19" s="28">
+        <v>0</v>
+      </c>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="24">
-        <v>17380.137404260553</v>
-      </c>
-      <c r="D20" s="16"/>
+      <c r="C20" s="11">
+        <v>5.7692307692307692</v>
+      </c>
+      <c r="D20" s="13">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="24">
-        <v>8670.1829613931368</v>
-      </c>
-      <c r="D21" s="16"/>
+      <c r="C21" s="11">
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="D21" s="13">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C22" s="11">
-        <v>5.7692307692307692</v>
+        <v>85.714285714285708</v>
       </c>
       <c r="D22" s="13">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C23" s="11">
-        <v>0.23076923076923078</v>
+        <v>14.285714285714285</v>
       </c>
       <c r="D23" s="13">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1359,103 +1381,63 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C24" s="11">
-        <v>85.714285714285708</v>
+        <v>5</v>
       </c>
       <c r="D24" s="13">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="11">
-        <v>14.285714285714285</v>
-      </c>
-      <c r="D25" s="13">
-        <v>50</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="11">
-        <v>5</v>
-      </c>
-      <c r="D26" s="13">
-        <v>5</v>
-      </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>36</v>
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="7">
+        <f>SUM(B29:B30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="7">
-        <f>SUM(B31:B32)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1486,7 +1468,7 @@
         <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1504,14 +1486,14 @@
       </c>
       <c r="B3" t="str">
         <f>portfolio_input!D3</f>
-        <v>The Proportional portfolio reflects a buildout of energy resources in the SJV consistent with the idea that the SJV contributes to the State's energy goals proportional to its resources. That proportionality is defined differently for each feedstock to commodity pathway and should be thought of as a guiding principle rather than a strict rule.</v>
+        <v>The Proportional portfolio reflects a buildout of energy resources in the SJV consistent with the idea that the SJV contributes to the State's energy goals proportional to its resources. That proportionality is defined differently for each feedstock to commodity pathway and should be thought of as a guiding principle rather than a strict rule. THIS PORTFOLIO ONLY USES BIOGAS TO PRODUCE BIOMETHANE FOR THE GAS GRID WHILE WE UPDATE THE MODEL.</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="26">
         <v>45322</v>
       </c>
     </row>
@@ -1521,7 +1503,7 @@
       </c>
       <c r="B5" t="str">
         <f>portfolio_input!D3</f>
-        <v>The Proportional portfolio reflects a buildout of energy resources in the SJV consistent with the idea that the SJV contributes to the State's energy goals proportional to its resources. That proportionality is defined differently for each feedstock to commodity pathway and should be thought of as a guiding principle rather than a strict rule.</v>
+        <v>The Proportional portfolio reflects a buildout of energy resources in the SJV consistent with the idea that the SJV contributes to the State's energy goals proportional to its resources. That proportionality is defined differently for each feedstock to commodity pathway and should be thought of as a guiding principle rather than a strict rule. THIS PORTFOLIO ONLY USES BIOGAS TO PRODUCE BIOMETHANE FOR THE GAS GRID WHILE WE UPDATE THE MODEL.</v>
       </c>
     </row>
   </sheetData>
@@ -2065,87 +2047,87 @@
       </c>
       <c r="G6" s="18">
         <f t="shared" si="1"/>
-        <v>1.0056196391600118</v>
+        <v>1.6326530612244898</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>2.0112392783200237</v>
+        <v>3.2653061224489797</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>3.0168589174800355</v>
+        <v>4.8979591836734695</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>4.0224785566400474</v>
+        <v>6.5306122448979593</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>5.0280981958000588</v>
+        <v>8.1632653061224492</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>6.0337178349600702</v>
+        <v>9.795918367346939</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>7.0393374741200816</v>
+        <v>11.428571428571429</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>8.044957113280093</v>
+        <v>13.061224489795919</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>9.0505767524401044</v>
+        <v>14.693877551020408</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>10.056196391600116</v>
+        <v>16.326530612244898</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>11.061816030760127</v>
+        <v>17.95918367346939</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>12.067435669920139</v>
+        <v>19.591836734693878</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>13.07305530908015</v>
+        <v>21.224489795918366</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>14.078674948240161</v>
+        <v>22.857142857142854</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>15.084294587400173</v>
+        <v>24.489795918367342</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>16.089914226560186</v>
+        <v>26.12244897959183</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>17.095533865720199</v>
+        <v>27.755102040816318</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>18.101153504880212</v>
+        <v>29.387755102040806</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>19.106773144040226</v>
+        <v>31.020408163265294</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>20.112392783200239</v>
+        <v>32.653061224489782</v>
       </c>
       <c r="AA6">
         <f>portfolio_input!C12*1000</f>
-        <v>21.118012422360248</v>
+        <v>34.285714285714285</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
@@ -2169,87 +2151,87 @@
       </c>
       <c r="G7" s="18">
         <f t="shared" si="1"/>
-        <v>0.16563146997929609</v>
+        <v>0.14365994845143032</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>0.33126293995859218</v>
+        <v>0.28731989690286064</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0.49689440993788825</v>
+        <v>0.43097984535429096</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0.66252587991718437</v>
+        <v>0.57463979380572128</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0.82815734989648049</v>
+        <v>0.71829974225715154</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0.99378881987577661</v>
+        <v>0.8619596907085818</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>1.1594202898550727</v>
+        <v>1.0056196391600121</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>1.3250517598343687</v>
+        <v>1.1492795876114423</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>1.4906832298136647</v>
+        <v>1.2929395360628726</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>1.6563146997929608</v>
+        <v>1.4365994845143029</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>1.8219461697722568</v>
+        <v>1.5802594329657331</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>1.9875776397515528</v>
+        <v>1.7239193814171634</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>2.1532091097308488</v>
+        <v>1.8675793298685937</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>2.318840579710145</v>
+        <v>2.0112392783200241</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>2.4844720496894412</v>
+        <v>2.1548992267714544</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>2.6501035196687375</v>
+        <v>2.2985591752228847</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>2.8157349896480337</v>
+        <v>2.4422191236743149</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>2.9813664596273299</v>
+        <v>2.5858790721257452</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>3.1469979296066262</v>
+        <v>2.7295390205771755</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>3.3126293995859224</v>
+        <v>2.8731989690286057</v>
       </c>
       <c r="AA7">
         <f>portfolio_input!C13*1000</f>
-        <v>3.4782608695652177</v>
+        <v>3.0168589174800369</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
@@ -2273,87 +2255,87 @@
       </c>
       <c r="G8" s="18">
         <f t="shared" si="1"/>
-        <v>0.7098491570541261</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>1.4196983141082522</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>2.1295474711623781</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>2.8393966282165044</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>3.5492457852706307</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>4.259094942324757</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>4.9689440993788834</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>5.6787932564330097</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>6.388642413487136</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>7.0984915705412623</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>7.8083407275953887</v>
+        <v>0</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>8.5181898846495141</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>9.2280390417036404</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>9.9378881987577667</v>
+        <v>0</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>10.647737355811893</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>11.357586512866019</v>
+        <v>0</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>12.067435669920146</v>
+        <v>0</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>12.777284826974272</v>
+        <v>0</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>13.487133984028398</v>
+        <v>0</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>14.196983141082525</v>
+        <v>0</v>
       </c>
       <c r="AA8">
         <f>portfolio_input!C14*1000</f>
-        <v>14.906832298136647</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
@@ -2375,89 +2357,89 @@
       <c r="F9" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="18" t="e">
         <f t="shared" si="1"/>
-        <v>2.3661638568470866E-2</v>
-      </c>
-      <c r="H9">
+        <v>#REF!</v>
+      </c>
+      <c r="H9" t="e">
         <f t="shared" si="2"/>
-        <v>4.7323277136941733E-2</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>7.0984915705412599E-2</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>9.4646554273883465E-2</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>0.11830819284235433</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>0.1419698314108252</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>0.16563146997929606</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="0"/>
-        <v>0.18929310854776693</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>0.2129547471162378</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0.23661638568470866</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="0"/>
-        <v>0.26027802425317953</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="0"/>
-        <v>0.2839396628216504</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="0"/>
-        <v>0.30760130139012126</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="0"/>
-        <v>0.33126293995859213</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="0"/>
-        <v>0.35492457852706299</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="0"/>
-        <v>0.37858621709553386</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="0"/>
-        <v>0.40224785566400473</v>
-      </c>
-      <c r="X9">
-        <f t="shared" si="0"/>
-        <v>0.42590949423247559</v>
-      </c>
-      <c r="Y9">
-        <f t="shared" si="0"/>
-        <v>0.44957113280094646</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="0"/>
-        <v>0.47323277136941733</v>
-      </c>
-      <c r="AA9">
-        <f>portfolio_input!C15*1000</f>
-        <v>0.49689440993788819</v>
+        <v>#REF!</v>
+      </c>
+      <c r="I9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="M9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="O9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="P9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="Q9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="R9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="S9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="T9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="U9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="V9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="W9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="X9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="Y9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="Z9" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AA9" t="e">
+        <f>portfolio_input!#REF!*1000</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -2560,7 +2542,7 @@
         <v>295238.09523809515</v>
       </c>
       <c r="AA10" s="18">
-        <f>portfolio_input!C16</f>
+        <f>portfolio_input!C15</f>
         <v>310000</v>
       </c>
     </row>
@@ -2664,7 +2646,7 @@
         <v>10476.190476190473</v>
       </c>
       <c r="AA11" s="18">
-        <f>portfolio_input!C17</f>
+        <f>portfolio_input!C16</f>
         <v>11000</v>
       </c>
     </row>
@@ -2689,87 +2671,87 @@
       </c>
       <c r="G12" s="18">
         <f t="shared" si="1"/>
-        <v>3325.7055682684972</v>
+        <v>5721.7847769028867</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>6651.4111365369945</v>
+        <v>11443.569553805773</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>9977.1167048054922</v>
+        <v>17165.354330708658</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>13302.822273073989</v>
+        <v>22887.139107611547</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>16628.527841342486</v>
+        <v>28608.923884514435</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>19954.233409610984</v>
+        <v>34330.708661417324</v>
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>23279.938977879483</v>
+        <v>40052.493438320213</v>
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>26605.644546147982</v>
+        <v>45774.278215223101</v>
       </c>
       <c r="O12">
         <f t="shared" si="0"/>
-        <v>29931.35011441648</v>
+        <v>51496.06299212599</v>
       </c>
       <c r="P12">
         <f t="shared" si="0"/>
-        <v>33257.055682684979</v>
+        <v>57217.847769028878</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
-        <v>36582.761250953474</v>
+        <v>62939.632545931767</v>
       </c>
       <c r="R12">
         <f t="shared" si="0"/>
-        <v>39908.466819221969</v>
+        <v>68661.417322834648</v>
       </c>
       <c r="S12">
         <f t="shared" si="0"/>
-        <v>43234.172387490464</v>
+        <v>74383.202099737537</v>
       </c>
       <c r="T12">
         <f t="shared" si="0"/>
-        <v>46559.877955758959</v>
+        <v>80104.986876640425</v>
       </c>
       <c r="U12">
         <f t="shared" si="0"/>
-        <v>49885.583524027454</v>
+        <v>85826.771653543314</v>
       </c>
       <c r="V12">
         <f t="shared" si="0"/>
-        <v>53211.289092295949</v>
+        <v>91548.556430446202</v>
       </c>
       <c r="W12">
         <f t="shared" si="0"/>
-        <v>56536.994660564444</v>
+        <v>97270.341207349091</v>
       </c>
       <c r="X12">
         <f t="shared" si="0"/>
-        <v>59862.700228832939</v>
+        <v>102992.12598425198</v>
       </c>
       <c r="Y12">
         <f t="shared" si="0"/>
-        <v>63188.405797101434</v>
+        <v>108713.91076115487</v>
       </c>
       <c r="Z12">
         <f t="shared" si="0"/>
-        <v>66514.111365369929</v>
+        <v>114435.69553805776</v>
       </c>
       <c r="AA12" s="18">
-        <f>portfolio_input!C18</f>
-        <v>69839.816933638445</v>
+        <f>portfolio_input!C17</f>
+        <v>120157.48031496063</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
@@ -2793,87 +2775,87 @@
       </c>
       <c r="G13" s="18">
         <f t="shared" si="1"/>
-        <v>1659.0476290218132</v>
+        <v>471.35984432151918</v>
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
-        <v>3318.0952580436265</v>
+        <v>942.71968864303835</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>4977.1428870654399</v>
+        <v>1414.0795329645575</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>6636.1905160872529</v>
+        <v>1885.4393772860767</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>8295.238145109066</v>
+        <v>2356.7992216075959</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>9954.2857741308799</v>
+        <v>2828.1590659291151</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>11613.333403152694</v>
+        <v>3299.5189102506342</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>13272.381032174508</v>
+        <v>3770.8787545721534</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>14931.428661196322</v>
+        <v>4242.238598893673</v>
       </c>
       <c r="P13">
         <f t="shared" si="0"/>
-        <v>16590.476290218136</v>
+        <v>4713.5984432151927</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
-        <v>18249.523919239949</v>
+        <v>5184.9582875367123</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>19908.571548261763</v>
+        <v>5656.3181318582319</v>
       </c>
       <c r="S13">
         <f t="shared" si="0"/>
-        <v>21567.619177283577</v>
+        <v>6127.6779761797516</v>
       </c>
       <c r="T13">
         <f t="shared" si="0"/>
-        <v>23226.666806305391</v>
+        <v>6599.0378205012712</v>
       </c>
       <c r="U13">
         <f t="shared" si="0"/>
-        <v>24885.714435327205</v>
+        <v>7070.3976648227908</v>
       </c>
       <c r="V13">
         <f t="shared" si="0"/>
-        <v>26544.762064349019</v>
+        <v>7541.7575091443105</v>
       </c>
       <c r="W13">
         <f t="shared" si="0"/>
-        <v>28203.809693370833</v>
+        <v>8013.1173534658301</v>
       </c>
       <c r="X13">
         <f t="shared" si="0"/>
-        <v>29862.857322392647</v>
+        <v>8484.4771977873497</v>
       </c>
       <c r="Y13">
         <f t="shared" si="0"/>
-        <v>31521.904951414461</v>
+        <v>8955.8370421088694</v>
       </c>
       <c r="Z13">
         <f t="shared" si="0"/>
-        <v>33180.952580436271</v>
+        <v>9427.196886430389</v>
       </c>
       <c r="AA13" s="18">
-        <f>portfolio_input!C19</f>
-        <v>34840.000209458078</v>
+        <f>portfolio_input!C18</f>
+        <v>9898.5567307519032</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
@@ -2897,87 +2879,87 @@
       </c>
       <c r="G14" s="18">
         <f t="shared" si="1"/>
-        <v>827.62559067907398</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>1655.251181358148</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>2482.8767720372221</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>3310.5023627162959</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>4138.1279533953702</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>4965.7535440744441</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>5793.379134753518</v>
+        <v>0</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>6621.0047254325918</v>
+        <v>0</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
-        <v>7448.6303161116657</v>
+        <v>0</v>
       </c>
       <c r="P14">
         <f t="shared" si="0"/>
-        <v>8276.2559067907405</v>
+        <v>0</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
-        <v>9103.8814974698143</v>
+        <v>0</v>
       </c>
       <c r="R14">
         <f t="shared" si="0"/>
-        <v>9931.5070881488882</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <f t="shared" si="0"/>
-        <v>10759.132678827962</v>
+        <v>0</v>
       </c>
       <c r="T14">
         <f t="shared" si="0"/>
-        <v>11586.758269507036</v>
+        <v>0</v>
       </c>
       <c r="U14">
         <f t="shared" si="0"/>
-        <v>12414.38386018611</v>
+        <v>0</v>
       </c>
       <c r="V14">
         <f t="shared" si="0"/>
-        <v>13242.009450865184</v>
+        <v>0</v>
       </c>
       <c r="W14">
         <f t="shared" si="0"/>
-        <v>14069.635041544258</v>
+        <v>0</v>
       </c>
       <c r="X14">
         <f t="shared" si="0"/>
-        <v>14897.260632223331</v>
+        <v>0</v>
       </c>
       <c r="Y14">
         <f t="shared" si="0"/>
-        <v>15724.886222902405</v>
+        <v>0</v>
       </c>
       <c r="Z14">
         <f t="shared" si="0"/>
-        <v>16552.511813581481</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="18">
-        <f>portfolio_input!C20</f>
-        <v>17380.137404260553</v>
+        <f>portfolio_input!C19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
@@ -2999,89 +2981,89 @@
       <c r="F15" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="18" t="e">
         <f t="shared" si="1"/>
-        <v>412.86585530443506</v>
-      </c>
-      <c r="H15">
+        <v>#REF!</v>
+      </c>
+      <c r="H15" t="e">
         <f t="shared" si="2"/>
-        <v>825.73171060887012</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>1238.5975659133051</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>1651.4634212177402</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>2064.3292765221754</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
-        <v>2477.1951318266106</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="0"/>
-        <v>2890.0609871310457</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="0"/>
-        <v>3302.9268424354809</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="0"/>
-        <v>3715.7926977399161</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>4128.6585530443508</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="0"/>
-        <v>4541.524408348786</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="0"/>
-        <v>4954.3902636532212</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="0"/>
-        <v>5367.2561189576563</v>
-      </c>
-      <c r="T15">
-        <f t="shared" si="0"/>
-        <v>5780.1219742620915</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="0"/>
-        <v>6192.9878295665267</v>
-      </c>
-      <c r="V15">
-        <f t="shared" si="0"/>
-        <v>6605.8536848709618</v>
-      </c>
-      <c r="W15">
-        <f t="shared" si="0"/>
-        <v>7018.719540175397</v>
-      </c>
-      <c r="X15">
-        <f t="shared" si="0"/>
-        <v>7431.5853954798322</v>
-      </c>
-      <c r="Y15">
-        <f t="shared" si="0"/>
-        <v>7844.4512507842674</v>
-      </c>
-      <c r="Z15">
-        <f t="shared" si="0"/>
-        <v>8257.3171060887016</v>
-      </c>
-      <c r="AA15" s="18">
-        <f>portfolio_input!C21</f>
-        <v>8670.1829613931368</v>
+        <v>#REF!</v>
+      </c>
+      <c r="I15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="M15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="O15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="P15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="Q15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="R15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="S15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="T15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="U15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="V15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="W15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="X15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="Y15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="Z15" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AA15" s="18" t="e">
+        <f>portfolio_input!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
@@ -3184,7 +3166,7 @@
         <v>5494.5054945054953</v>
       </c>
       <c r="AA16" s="18">
-        <f>portfolio_input!C22*1000</f>
+        <f>portfolio_input!C20*1000</f>
         <v>5769.2307692307695</v>
       </c>
     </row>
@@ -3288,7 +3270,7 @@
         <v>219.78021978021971</v>
       </c>
       <c r="AA17" s="18">
-        <f>portfolio_input!C23*1000</f>
+        <f>portfolio_input!C21*1000</f>
         <v>230.76923076923077</v>
       </c>
     </row>
@@ -3392,7 +3374,7 @@
         <v>81632.653061224526</v>
       </c>
       <c r="AA18">
-        <f>portfolio_input!C24*1000</f>
+        <f>portfolio_input!C22*1000</f>
         <v>85714.28571428571</v>
       </c>
     </row>
@@ -3496,7 +3478,7 @@
         <v>13605.442176870747</v>
       </c>
       <c r="AA19">
-        <f>portfolio_input!C25*1000</f>
+        <f>portfolio_input!C23*1000</f>
         <v>14285.714285714284</v>
       </c>
     </row>
@@ -3600,7 +3582,7 @@
         <v>4761.9047619047633</v>
       </c>
       <c r="AA20">
-        <f>portfolio_input!C26*1000</f>
+        <f>portfolio_input!C24*1000</f>
         <v>5000</v>
       </c>
     </row>
@@ -3611,10 +3593,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A302D73-9F74-D647-9FC8-5951743D164F}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3909,143 +3891,285 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="25">
+        <v>1</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25">
+        <v>1</v>
+      </c>
+      <c r="F5" s="25">
+        <v>1</v>
+      </c>
+      <c r="G5" s="25">
+        <v>1</v>
+      </c>
+      <c r="H5" s="25">
+        <v>1</v>
+      </c>
+      <c r="I5" s="25">
+        <v>1</v>
+      </c>
+      <c r="J5" s="25">
+        <v>1</v>
+      </c>
+      <c r="K5" s="25">
+        <v>1</v>
+      </c>
+      <c r="L5" s="25">
+        <v>1</v>
+      </c>
+      <c r="M5" s="25">
+        <v>1</v>
+      </c>
+      <c r="N5" s="25">
+        <v>1</v>
+      </c>
+      <c r="O5" s="25">
+        <v>1</v>
+      </c>
+      <c r="P5" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="25">
+        <v>1</v>
+      </c>
+      <c r="R5" s="25">
+        <v>1</v>
+      </c>
+      <c r="S5" s="25">
+        <v>1</v>
+      </c>
+      <c r="T5" s="25">
+        <v>1</v>
+      </c>
+      <c r="U5" s="25">
+        <v>1</v>
+      </c>
+      <c r="V5" s="25">
+        <v>1</v>
+      </c>
+      <c r="W5" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="25">
-        <v>1</v>
-      </c>
-      <c r="D5" s="25">
-        <v>1</v>
-      </c>
-      <c r="E5" s="25">
-        <v>1</v>
-      </c>
-      <c r="F5" s="25">
-        <v>1</v>
-      </c>
-      <c r="G5" s="25">
-        <v>1</v>
-      </c>
-      <c r="H5" s="25">
-        <v>1</v>
-      </c>
-      <c r="I5" s="25">
-        <v>1</v>
-      </c>
-      <c r="J5" s="25">
-        <v>1</v>
-      </c>
-      <c r="K5" s="25">
-        <v>1</v>
-      </c>
-      <c r="L5" s="25">
-        <v>1</v>
-      </c>
-      <c r="M5" s="25">
-        <v>1</v>
-      </c>
-      <c r="N5" s="25">
-        <v>1</v>
-      </c>
-      <c r="O5" s="25">
-        <v>1</v>
-      </c>
-      <c r="P5" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="25">
-        <v>1</v>
-      </c>
-      <c r="R5" s="25">
-        <v>1</v>
-      </c>
-      <c r="S5" s="25">
-        <v>1</v>
-      </c>
-      <c r="T5" s="25">
-        <v>1</v>
-      </c>
-      <c r="U5" s="25">
-        <v>1</v>
-      </c>
-      <c r="V5" s="25">
-        <v>1</v>
-      </c>
-      <c r="W5" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="25">
-        <v>1</v>
-      </c>
-      <c r="D6" s="25">
-        <v>1</v>
-      </c>
-      <c r="E6" s="25">
-        <v>1</v>
-      </c>
-      <c r="F6" s="25">
-        <v>1</v>
-      </c>
-      <c r="G6" s="25">
-        <v>1</v>
-      </c>
-      <c r="H6" s="25">
-        <v>1</v>
-      </c>
-      <c r="I6" s="25">
-        <v>1</v>
-      </c>
-      <c r="J6" s="25">
-        <v>1</v>
-      </c>
-      <c r="K6" s="25">
-        <v>1</v>
-      </c>
-      <c r="L6" s="25">
-        <v>1</v>
-      </c>
-      <c r="M6" s="25">
-        <v>1</v>
-      </c>
-      <c r="N6" s="25">
-        <v>1</v>
-      </c>
-      <c r="O6" s="25">
-        <v>1</v>
-      </c>
-      <c r="P6" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="25">
-        <v>1</v>
-      </c>
-      <c r="R6" s="25">
-        <v>1</v>
-      </c>
-      <c r="S6" s="25">
-        <v>1</v>
-      </c>
-      <c r="T6" s="25">
-        <v>1</v>
-      </c>
-      <c r="U6" s="25">
-        <v>1</v>
-      </c>
-      <c r="V6" s="25">
-        <v>1</v>
-      </c>
-      <c r="W6" s="25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
         <v>1</v>
       </c>
     </row>
@@ -4056,7 +4180,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCD9FC6-402B-8D4F-AF23-A8506C6A96EC}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16:D16"/>
@@ -4129,8 +4253,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="C4" s="19">
+        <f>C2/(C2+D2)</f>
+        <v>0.8582677165354331</v>
+      </c>
+      <c r="D4" s="19">
+        <f>1-C4</f>
+        <v>0.1417322834645669</v>
+      </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="H4" s="19"/>
@@ -4216,8 +4346,8 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="D9" s="19">
-        <f>D7/(C7+D7)</f>
-        <v>0.14285714285714285</v>
+        <f>1-C9</f>
+        <v>0.1428571428571429</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
@@ -4296,63 +4426,85 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="C14">
+        <f>B13*C9</f>
+        <v>3.4285714285714287E-2</v>
+      </c>
+      <c r="D14">
+        <f>C13*D9</f>
+        <v>3.0168589174800367E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B15" s="5">
         <v>140000</v>
       </c>
-      <c r="C14">
-        <f>B14*$C3</f>
+      <c r="C15">
+        <f>B15*$C3</f>
         <v>69839.816933638445</v>
       </c>
-      <c r="D14">
-        <f>C14*$C3</f>
+      <c r="D15">
+        <f>C15*$C3</f>
         <v>34840.000209458078</v>
       </c>
-      <c r="E14">
-        <f>D14*$C3</f>
+      <c r="E15">
+        <f>D15*$C3</f>
         <v>17380.137404260553</v>
       </c>
-      <c r="F14">
-        <f>E14*$C3</f>
+      <c r="F15">
+        <f>E15*$C3</f>
         <v>8670.1829613931368</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16">
+        <f>B15*C4</f>
+        <v>120157.48031496063</v>
+      </c>
+      <c r="D16">
+        <f>C15*D4</f>
+        <v>9898.5567307519032</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>90</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>6</v>
       </c>
-      <c r="E15">
-        <f>$B15*E6</f>
+      <c r="E17">
+        <f>$B17*E6</f>
         <v>5.7692307692307692</v>
       </c>
-      <c r="F15">
-        <f>$B15*F6</f>
+      <c r="F17">
+        <f>$B17*F6</f>
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>91</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>100</v>
       </c>
-      <c r="C16">
-        <f>$B16*C9</f>
+      <c r="C18">
+        <f>$B18*C9</f>
         <v>85.714285714285708</v>
       </c>
-      <c r="D16">
-        <f>$B16*D9</f>
-        <v>14.285714285714285</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D27">
+      <c r="D18">
+        <f>$B18*D9</f>
+        <v>14.28571428571429</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D29">
         <f>215000-193500</f>
         <v>21500</v>
       </c>

</xml_diff>